<commit_message>
Added refs to extended toolkit and windows forms, modified imports and main form
</commit_message>
<xml_diff>
--- a/Impilo App/Templates/Format2Hypertension.xlsx
+++ b/Impilo App/Templates/Format2Hypertension.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhaskins\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhaskins\Source\Repos\WoodsFoun_Project\Impilo App\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="NCD Indicators" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -264,12 +264,6 @@
     <t>7b.  No. not diagnosed and not put on treatment or further clinic visit  [F]</t>
   </si>
   <si>
-    <t>23a.  No. not diagnosed &amp; referred by nurse for 1/12 clinic visit</t>
-  </si>
-  <si>
-    <t>23b.  No. not diagnosed and not put on treatment or further clinic visit</t>
-  </si>
-  <si>
     <t>No. of feet examined, no. with neurophy detected (NB: Diabetes only)</t>
   </si>
   <si>
@@ -527,6 +521,12 @@
   </si>
   <si>
     <t>Level of HbA1c, cholesterol,creatinine done annually</t>
+  </si>
+  <si>
+    <t>22a.  No. not diagnosed &amp; referred by nurse for 1/12 clinic visit</t>
+  </si>
+  <si>
+    <t>22b.  No. not diagnosed and not put on treatment or further clinic visit</t>
   </si>
 </sst>
 </file>
@@ -1454,6 +1454,18 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1463,56 +1475,44 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="89">
@@ -1887,10 +1887,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AY32"/>
+  <dimension ref="A2:AY33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1932,333 +1932,230 @@
     <col min="36" max="51" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" ht="27" customHeight="1">
-      <c r="A1" s="19"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
-      <c r="W1" s="21"/>
-      <c r="X1" s="21"/>
-      <c r="Y1" s="21"/>
-      <c r="Z1" s="21"/>
-      <c r="AA1" s="21"/>
-      <c r="AB1" s="21"/>
-      <c r="AC1" s="21"/>
-      <c r="AD1" s="21"/>
-      <c r="AE1" s="21"/>
-      <c r="AF1" s="21"/>
-      <c r="AG1" s="21"/>
-      <c r="AH1" s="21"/>
-      <c r="AI1" s="21"/>
+    <row r="2" spans="1:51" ht="27" customHeight="1">
+      <c r="A2" s="19"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="21"/>
+      <c r="U2" s="21"/>
+      <c r="V2" s="21"/>
+      <c r="W2" s="21"/>
+      <c r="X2" s="21"/>
+      <c r="Y2" s="21"/>
+      <c r="Z2" s="21"/>
+      <c r="AA2" s="21"/>
+      <c r="AB2" s="21"/>
+      <c r="AC2" s="21"/>
+      <c r="AD2" s="21"/>
+      <c r="AE2" s="21"/>
+      <c r="AF2" s="21"/>
+      <c r="AG2" s="21"/>
+      <c r="AH2" s="21"/>
+      <c r="AI2" s="21"/>
     </row>
-    <row r="2" spans="1:51" s="17" customFormat="1" ht="27" customHeight="1">
-      <c r="A2" s="38"/>
-      <c r="B2" s="120" t="s">
-        <v>87</v>
-      </c>
-      <c r="C2" s="121" t="s">
+    <row r="3" spans="1:51" s="17" customFormat="1" ht="27" customHeight="1">
+      <c r="A3" s="38"/>
+      <c r="B3" s="120" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="121" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="121"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
-      <c r="U2" s="24"/>
-      <c r="V2" s="25"/>
-      <c r="W2" s="24"/>
-      <c r="X2" s="24"/>
-      <c r="Y2" s="24"/>
-      <c r="Z2" s="24"/>
-      <c r="AA2" s="24"/>
-      <c r="AB2" s="24"/>
-      <c r="AC2" s="24"/>
-      <c r="AD2" s="24"/>
-      <c r="AE2" s="24"/>
-      <c r="AF2" s="24"/>
-      <c r="AG2" s="24"/>
-      <c r="AH2" s="24"/>
-      <c r="AI2" s="24"/>
-      <c r="AJ2" s="16"/>
-      <c r="AK2" s="16"/>
-      <c r="AL2" s="16"/>
-      <c r="AM2" s="16"/>
-      <c r="AN2" s="16"/>
-      <c r="AO2" s="16"/>
-      <c r="AP2" s="16"/>
-      <c r="AQ2" s="16"/>
-      <c r="AR2" s="16"/>
-      <c r="AS2" s="16"/>
-      <c r="AT2" s="16"/>
-      <c r="AU2" s="16"/>
-      <c r="AV2" s="16"/>
-      <c r="AW2" s="16"/>
-      <c r="AX2" s="16"/>
-      <c r="AY2" s="16"/>
+      <c r="D3" s="121"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
+      <c r="Q3" s="24"/>
+      <c r="R3" s="24"/>
+      <c r="S3" s="24"/>
+      <c r="T3" s="24"/>
+      <c r="U3" s="24"/>
+      <c r="V3" s="25"/>
+      <c r="W3" s="24"/>
+      <c r="X3" s="24"/>
+      <c r="Y3" s="24"/>
+      <c r="Z3" s="24"/>
+      <c r="AA3" s="24"/>
+      <c r="AB3" s="24"/>
+      <c r="AC3" s="24"/>
+      <c r="AD3" s="24"/>
+      <c r="AE3" s="24"/>
+      <c r="AF3" s="24"/>
+      <c r="AG3" s="24"/>
+      <c r="AH3" s="24"/>
+      <c r="AI3" s="24"/>
+      <c r="AJ3" s="16"/>
+      <c r="AK3" s="16"/>
+      <c r="AL3" s="16"/>
+      <c r="AM3" s="16"/>
+      <c r="AN3" s="16"/>
+      <c r="AO3" s="16"/>
+      <c r="AP3" s="16"/>
+      <c r="AQ3" s="16"/>
+      <c r="AR3" s="16"/>
+      <c r="AS3" s="16"/>
+      <c r="AT3" s="16"/>
+      <c r="AU3" s="16"/>
+      <c r="AV3" s="16"/>
+      <c r="AW3" s="16"/>
+      <c r="AX3" s="16"/>
+      <c r="AY3" s="16"/>
     </row>
-    <row r="3" spans="1:51" s="1" customFormat="1" ht="41.1" customHeight="1">
-      <c r="A3" s="32"/>
-      <c r="B3" s="45" t="s">
+    <row r="4" spans="1:51" s="1" customFormat="1" ht="41.1" customHeight="1">
+      <c r="A4" s="32"/>
+      <c r="B4" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="99" t="s">
+      <c r="C4" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="100" t="s">
+      <c r="D4" s="100" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="100" t="s">
+      <c r="E4" s="100" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="100" t="s">
+      <c r="F4" s="100" t="s">
         <v>59</v>
       </c>
-      <c r="G3" s="101" t="s">
-        <v>85</v>
-      </c>
-      <c r="H3" s="100" t="s">
+      <c r="G4" s="101" t="s">
+        <v>83</v>
+      </c>
+      <c r="H4" s="100" t="s">
         <v>75</v>
       </c>
-      <c r="I3" s="142" t="s">
-        <v>80</v>
-      </c>
-      <c r="J3" s="143"/>
-      <c r="K3" s="100" t="s">
+      <c r="I4" s="139" t="s">
+        <v>78</v>
+      </c>
+      <c r="J4" s="140"/>
+      <c r="K4" s="100" t="s">
         <v>61</v>
       </c>
-      <c r="L3" s="142" t="s">
+      <c r="L4" s="139" t="s">
         <v>68</v>
       </c>
-      <c r="M3" s="152"/>
-      <c r="N3" s="152"/>
-      <c r="O3" s="143"/>
-      <c r="P3" s="142" t="s">
+      <c r="M4" s="149"/>
+      <c r="N4" s="149"/>
+      <c r="O4" s="140"/>
+      <c r="P4" s="139" t="s">
         <v>74</v>
       </c>
-      <c r="Q3" s="143"/>
-      <c r="R3" s="142" t="s">
+      <c r="Q4" s="140"/>
+      <c r="R4" s="139" t="s">
         <v>72</v>
       </c>
-      <c r="S3" s="143"/>
-      <c r="T3" s="142" t="s">
+      <c r="S4" s="140"/>
+      <c r="T4" s="139" t="s">
         <v>73</v>
       </c>
-      <c r="U3" s="143"/>
-      <c r="V3" s="100" t="s">
-        <v>117</v>
-      </c>
-      <c r="W3" s="142" t="s">
+      <c r="U4" s="140"/>
+      <c r="V4" s="100" t="s">
+        <v>115</v>
+      </c>
+      <c r="W4" s="139" t="s">
         <v>22</v>
       </c>
-      <c r="X3" s="143"/>
-      <c r="Y3" s="142" t="s">
+      <c r="X4" s="140"/>
+      <c r="Y4" s="139" t="s">
         <v>25</v>
       </c>
-      <c r="Z3" s="143"/>
-      <c r="AA3" s="142" t="s">
+      <c r="Z4" s="140"/>
+      <c r="AA4" s="139" t="s">
         <v>28</v>
       </c>
-      <c r="AB3" s="143"/>
-      <c r="AC3" s="142" t="s">
+      <c r="AB4" s="140"/>
+      <c r="AC4" s="139" t="s">
         <v>31</v>
       </c>
-      <c r="AD3" s="143"/>
-      <c r="AE3" s="142" t="s">
+      <c r="AD4" s="140"/>
+      <c r="AE4" s="139" t="s">
         <v>34</v>
       </c>
-      <c r="AF3" s="143"/>
-      <c r="AG3" s="142" t="s">
+      <c r="AF4" s="140"/>
+      <c r="AG4" s="139" t="s">
         <v>71</v>
       </c>
-      <c r="AH3" s="143"/>
-      <c r="AI3" s="39"/>
-      <c r="AJ3" s="2"/>
-      <c r="AK3" s="2"/>
-      <c r="AL3" s="2"/>
-      <c r="AM3" s="2"/>
-      <c r="AN3" s="2"/>
-      <c r="AO3" s="2"/>
-      <c r="AP3" s="2"/>
-      <c r="AQ3" s="2"/>
-      <c r="AR3" s="2"/>
-      <c r="AS3" s="2"/>
-      <c r="AT3" s="2"/>
-      <c r="AU3" s="2"/>
-      <c r="AV3" s="2"/>
-      <c r="AW3" s="2"/>
-      <c r="AX3" s="2"/>
-      <c r="AY3" s="2"/>
+      <c r="AH4" s="140"/>
+      <c r="AI4" s="39"/>
+      <c r="AJ4" s="2"/>
+      <c r="AK4" s="2"/>
+      <c r="AL4" s="2"/>
+      <c r="AM4" s="2"/>
+      <c r="AN4" s="2"/>
+      <c r="AO4" s="2"/>
+      <c r="AP4" s="2"/>
+      <c r="AQ4" s="2"/>
+      <c r="AR4" s="2"/>
+      <c r="AS4" s="2"/>
+      <c r="AT4" s="2"/>
+      <c r="AU4" s="2"/>
+      <c r="AV4" s="2"/>
+      <c r="AW4" s="2"/>
+      <c r="AX4" s="2"/>
+      <c r="AY4" s="2"/>
     </row>
-    <row r="4" spans="1:51" s="14" customFormat="1" ht="21.95" customHeight="1">
-      <c r="A4" s="33"/>
-      <c r="B4" s="46" t="s">
+    <row r="5" spans="1:51" s="14" customFormat="1" ht="21.95" customHeight="1">
+      <c r="A5" s="33"/>
+      <c r="B5" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="102"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="103"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="104"/>
-      <c r="M4" s="105"/>
-      <c r="N4" s="106"/>
-      <c r="O4" s="105"/>
-      <c r="P4" s="104"/>
-      <c r="Q4" s="105"/>
-      <c r="R4" s="104"/>
-      <c r="S4" s="105"/>
-      <c r="T4" s="104"/>
-      <c r="U4" s="105"/>
-      <c r="V4" s="45"/>
-      <c r="W4" s="104"/>
-      <c r="X4" s="105"/>
-      <c r="Y4" s="104"/>
-      <c r="Z4" s="105"/>
-      <c r="AA4" s="104"/>
-      <c r="AB4" s="105"/>
-      <c r="AC4" s="104"/>
-      <c r="AD4" s="105"/>
-      <c r="AE4" s="104"/>
-      <c r="AF4" s="105"/>
-      <c r="AG4" s="104"/>
-      <c r="AH4" s="106"/>
-      <c r="AI4" s="40"/>
-      <c r="AJ4" s="4"/>
-      <c r="AK4" s="4"/>
-      <c r="AL4" s="4"/>
-      <c r="AM4" s="4"/>
-      <c r="AN4" s="4"/>
-      <c r="AO4" s="4"/>
-      <c r="AP4" s="4"/>
-      <c r="AQ4" s="4"/>
-      <c r="AR4" s="4"/>
-      <c r="AS4" s="4"/>
-      <c r="AT4" s="4"/>
-      <c r="AU4" s="4"/>
-      <c r="AV4" s="4"/>
-      <c r="AW4" s="4"/>
-      <c r="AX4" s="4"/>
-      <c r="AY4" s="4"/>
-    </row>
-    <row r="5" spans="1:51" s="14" customFormat="1" ht="52.5" customHeight="1">
-      <c r="A5" s="33"/>
-      <c r="B5" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="107"/>
-      <c r="D5" s="108"/>
-      <c r="E5" s="108"/>
-      <c r="F5" s="108"/>
-      <c r="G5" s="108"/>
-      <c r="H5" s="108"/>
-      <c r="I5" s="109" t="s">
-        <v>81</v>
-      </c>
-      <c r="J5" s="109" t="s">
-        <v>76</v>
-      </c>
-      <c r="K5" s="108"/>
-      <c r="L5" s="110" t="s">
-        <v>12</v>
-      </c>
-      <c r="M5" s="110" t="s">
-        <v>13</v>
-      </c>
-      <c r="N5" s="110" t="s">
-        <v>14</v>
-      </c>
-      <c r="O5" s="110" t="s">
-        <v>15</v>
-      </c>
-      <c r="P5" s="110" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q5" s="110" t="s">
-        <v>17</v>
-      </c>
-      <c r="R5" s="110" t="s">
-        <v>18</v>
-      </c>
-      <c r="S5" s="110" t="s">
-        <v>19</v>
-      </c>
-      <c r="T5" s="110" t="s">
-        <v>20</v>
-      </c>
-      <c r="U5" s="110" t="s">
-        <v>21</v>
-      </c>
-      <c r="V5" s="108"/>
-      <c r="W5" s="110" t="s">
-        <v>23</v>
-      </c>
-      <c r="X5" s="110" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y5" s="110" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z5" s="110" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA5" s="110" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB5" s="110" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC5" s="110" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD5" s="110" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE5" s="110" t="s">
-        <v>35</v>
-      </c>
-      <c r="AF5" s="110" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG5" s="110" t="s">
-        <v>37</v>
-      </c>
-      <c r="AH5" s="111" t="s">
-        <v>38</v>
-      </c>
+      <c r="C5" s="102"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="103"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="104"/>
+      <c r="M5" s="105"/>
+      <c r="N5" s="106"/>
+      <c r="O5" s="105"/>
+      <c r="P5" s="104"/>
+      <c r="Q5" s="105"/>
+      <c r="R5" s="104"/>
+      <c r="S5" s="105"/>
+      <c r="T5" s="104"/>
+      <c r="U5" s="105"/>
+      <c r="V5" s="45"/>
+      <c r="W5" s="104"/>
+      <c r="X5" s="105"/>
+      <c r="Y5" s="104"/>
+      <c r="Z5" s="105"/>
+      <c r="AA5" s="104"/>
+      <c r="AB5" s="105"/>
+      <c r="AC5" s="104"/>
+      <c r="AD5" s="105"/>
+      <c r="AE5" s="104"/>
+      <c r="AF5" s="105"/>
+      <c r="AG5" s="104"/>
+      <c r="AH5" s="106"/>
       <c r="AI5" s="40"/>
       <c r="AJ5" s="4"/>
       <c r="AK5" s="4"/>
@@ -2277,43 +2174,91 @@
       <c r="AX5" s="4"/>
       <c r="AY5" s="4"/>
     </row>
-    <row r="6" spans="1:51" s="14" customFormat="1" ht="24" customHeight="1">
+    <row r="6" spans="1:51" s="14" customFormat="1" ht="52.5" customHeight="1">
       <c r="A6" s="33"/>
-      <c r="B6" s="46" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="103"/>
-      <c r="D6" s="103"/>
-      <c r="E6" s="103"/>
-      <c r="F6" s="103"/>
-      <c r="G6" s="103"/>
-      <c r="H6" s="103"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="103"/>
-      <c r="L6" s="111"/>
-      <c r="M6" s="111"/>
-      <c r="N6" s="111"/>
-      <c r="O6" s="111"/>
-      <c r="P6" s="111"/>
-      <c r="Q6" s="111"/>
-      <c r="R6" s="111"/>
-      <c r="S6" s="111"/>
-      <c r="T6" s="111"/>
-      <c r="U6" s="111"/>
-      <c r="V6" s="103"/>
-      <c r="W6" s="111"/>
-      <c r="X6" s="111"/>
-      <c r="Y6" s="111"/>
-      <c r="Z6" s="111"/>
-      <c r="AA6" s="111"/>
-      <c r="AB6" s="111"/>
-      <c r="AC6" s="111"/>
-      <c r="AD6" s="111"/>
-      <c r="AE6" s="111"/>
-      <c r="AF6" s="111"/>
-      <c r="AG6" s="111"/>
-      <c r="AH6" s="111"/>
+      <c r="B6" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="107"/>
+      <c r="D6" s="108"/>
+      <c r="E6" s="108"/>
+      <c r="F6" s="108"/>
+      <c r="G6" s="108"/>
+      <c r="H6" s="108"/>
+      <c r="I6" s="109" t="s">
+        <v>79</v>
+      </c>
+      <c r="J6" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="K6" s="108"/>
+      <c r="L6" s="110" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6" s="110" t="s">
+        <v>13</v>
+      </c>
+      <c r="N6" s="110" t="s">
+        <v>14</v>
+      </c>
+      <c r="O6" s="110" t="s">
+        <v>15</v>
+      </c>
+      <c r="P6" s="110" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q6" s="110" t="s">
+        <v>17</v>
+      </c>
+      <c r="R6" s="110" t="s">
+        <v>18</v>
+      </c>
+      <c r="S6" s="110" t="s">
+        <v>19</v>
+      </c>
+      <c r="T6" s="110" t="s">
+        <v>20</v>
+      </c>
+      <c r="U6" s="110" t="s">
+        <v>21</v>
+      </c>
+      <c r="V6" s="108"/>
+      <c r="W6" s="110" t="s">
+        <v>23</v>
+      </c>
+      <c r="X6" s="110" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y6" s="110" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z6" s="110" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA6" s="110" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB6" s="110" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC6" s="110" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD6" s="110" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE6" s="110" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF6" s="110" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG6" s="110" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH6" s="111" t="s">
+        <v>38</v>
+      </c>
       <c r="AI6" s="40"/>
       <c r="AJ6" s="4"/>
       <c r="AK6" s="4"/>
@@ -2332,422 +2277,374 @@
       <c r="AX6" s="4"/>
       <c r="AY6" s="4"/>
     </row>
-    <row r="7" spans="1:51" s="15" customFormat="1" ht="25.5">
-      <c r="A7" s="34"/>
-      <c r="B7" s="112" t="s">
+    <row r="7" spans="1:51" s="14" customFormat="1" ht="24" customHeight="1">
+      <c r="A7" s="33"/>
+      <c r="B7" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="103"/>
+      <c r="D7" s="103"/>
+      <c r="E7" s="103"/>
+      <c r="F7" s="103"/>
+      <c r="G7" s="103"/>
+      <c r="H7" s="103"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="103"/>
+      <c r="L7" s="111"/>
+      <c r="M7" s="111"/>
+      <c r="N7" s="111"/>
+      <c r="O7" s="111"/>
+      <c r="P7" s="111"/>
+      <c r="Q7" s="111"/>
+      <c r="R7" s="111"/>
+      <c r="S7" s="111"/>
+      <c r="T7" s="111"/>
+      <c r="U7" s="111"/>
+      <c r="V7" s="103"/>
+      <c r="W7" s="111"/>
+      <c r="X7" s="111"/>
+      <c r="Y7" s="111"/>
+      <c r="Z7" s="111"/>
+      <c r="AA7" s="111"/>
+      <c r="AB7" s="111"/>
+      <c r="AC7" s="111"/>
+      <c r="AD7" s="111"/>
+      <c r="AE7" s="111"/>
+      <c r="AF7" s="111"/>
+      <c r="AG7" s="111"/>
+      <c r="AH7" s="111"/>
+      <c r="AI7" s="40"/>
+      <c r="AJ7" s="4"/>
+      <c r="AK7" s="4"/>
+      <c r="AL7" s="4"/>
+      <c r="AM7" s="4"/>
+      <c r="AN7" s="4"/>
+      <c r="AO7" s="4"/>
+      <c r="AP7" s="4"/>
+      <c r="AQ7" s="4"/>
+      <c r="AR7" s="4"/>
+      <c r="AS7" s="4"/>
+      <c r="AT7" s="4"/>
+      <c r="AU7" s="4"/>
+      <c r="AV7" s="4"/>
+      <c r="AW7" s="4"/>
+      <c r="AX7" s="4"/>
+      <c r="AY7" s="4"/>
+    </row>
+    <row r="8" spans="1:51" s="15" customFormat="1" ht="25.5">
+      <c r="A8" s="34"/>
+      <c r="B8" s="112" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="113" t="s">
+      <c r="C8" s="113" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="112" t="s">
+      <c r="D8" s="112" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="112" t="s">
+      <c r="E8" s="112" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="112" t="s">
+      <c r="F8" s="112" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="112"/>
-      <c r="H7" s="114" t="s">
+      <c r="G8" s="112"/>
+      <c r="H8" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="I7" s="114" t="s">
+      <c r="I8" s="114" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="114" t="s">
+      <c r="J8" s="114" t="s">
         <v>4</v>
       </c>
-      <c r="K7" s="112" t="s">
+      <c r="K8" s="112" t="s">
         <v>5</v>
       </c>
-      <c r="L7" s="144" t="s">
+      <c r="L8" s="141" t="s">
         <v>5</v>
       </c>
-      <c r="M7" s="144"/>
-      <c r="N7" s="144"/>
-      <c r="O7" s="144"/>
-      <c r="P7" s="144" t="s">
+      <c r="M8" s="141"/>
+      <c r="N8" s="141"/>
+      <c r="O8" s="141"/>
+      <c r="P8" s="141" t="s">
         <v>5</v>
       </c>
-      <c r="Q7" s="144"/>
-      <c r="R7" s="144" t="s">
+      <c r="Q8" s="141"/>
+      <c r="R8" s="141" t="s">
         <v>6</v>
       </c>
-      <c r="S7" s="144"/>
-      <c r="T7" s="144" t="s">
+      <c r="S8" s="141"/>
+      <c r="T8" s="141" t="s">
         <v>7</v>
       </c>
-      <c r="U7" s="144"/>
-      <c r="V7" s="114" t="s">
+      <c r="U8" s="141"/>
+      <c r="V8" s="114" t="s">
         <v>5</v>
       </c>
-      <c r="W7" s="144" t="s">
+      <c r="W8" s="141" t="s">
         <v>8</v>
       </c>
-      <c r="X7" s="144"/>
-      <c r="Y7" s="144" t="s">
+      <c r="X8" s="141"/>
+      <c r="Y8" s="141" t="s">
         <v>8</v>
       </c>
-      <c r="Z7" s="144"/>
-      <c r="AA7" s="144" t="s">
+      <c r="Z8" s="141"/>
+      <c r="AA8" s="141" t="s">
         <v>8</v>
       </c>
-      <c r="AB7" s="144"/>
-      <c r="AC7" s="144" t="s">
+      <c r="AB8" s="141"/>
+      <c r="AC8" s="141" t="s">
         <v>8</v>
       </c>
-      <c r="AD7" s="144"/>
-      <c r="AE7" s="144" t="s">
+      <c r="AD8" s="141"/>
+      <c r="AE8" s="141" t="s">
         <v>8</v>
       </c>
-      <c r="AF7" s="144"/>
-      <c r="AG7" s="144" t="s">
+      <c r="AF8" s="141"/>
+      <c r="AG8" s="141" t="s">
         <v>8</v>
       </c>
-      <c r="AH7" s="144"/>
-      <c r="AI7" s="41"/>
-      <c r="AJ7" s="7"/>
-      <c r="AK7" s="7"/>
-      <c r="AL7" s="7"/>
-      <c r="AM7" s="7"/>
-      <c r="AN7" s="7"/>
-      <c r="AO7" s="7"/>
-      <c r="AP7" s="7"/>
-      <c r="AQ7" s="7"/>
-      <c r="AR7" s="7"/>
-      <c r="AS7" s="7"/>
-      <c r="AT7" s="7"/>
-      <c r="AU7" s="7"/>
-      <c r="AV7" s="7"/>
-      <c r="AW7" s="7"/>
-      <c r="AX7" s="7"/>
-      <c r="AY7" s="7"/>
+      <c r="AH8" s="141"/>
+      <c r="AI8" s="41"/>
+      <c r="AJ8" s="7"/>
+      <c r="AK8" s="7"/>
+      <c r="AL8" s="7"/>
+      <c r="AM8" s="7"/>
+      <c r="AN8" s="7"/>
+      <c r="AO8" s="7"/>
+      <c r="AP8" s="7"/>
+      <c r="AQ8" s="7"/>
+      <c r="AR8" s="7"/>
+      <c r="AS8" s="7"/>
+      <c r="AT8" s="7"/>
+      <c r="AU8" s="7"/>
+      <c r="AV8" s="7"/>
+      <c r="AW8" s="7"/>
+      <c r="AX8" s="7"/>
+      <c r="AY8" s="7"/>
     </row>
-    <row r="8" spans="1:51" s="12" customFormat="1" ht="102" customHeight="1">
-      <c r="A8" s="26"/>
-      <c r="B8" s="115" t="s">
+    <row r="9" spans="1:51" s="12" customFormat="1" ht="102" customHeight="1">
+      <c r="A9" s="26"/>
+      <c r="B9" s="115" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="116" t="s">
-        <v>116</v>
-      </c>
-      <c r="D8" s="116" t="s">
+      <c r="C9" s="116" t="s">
+        <v>114</v>
+      </c>
+      <c r="D9" s="116" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="116" t="s">
+      <c r="E9" s="116" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" s="116" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" s="116" t="s">
         <v>84</v>
       </c>
-      <c r="F8" s="116" t="s">
-        <v>70</v>
-      </c>
-      <c r="G8" s="116" t="s">
-        <v>86</v>
-      </c>
-      <c r="H8" s="116" t="s">
-        <v>82</v>
-      </c>
-      <c r="I8" s="116" t="s">
-        <v>83</v>
-      </c>
-      <c r="J8" s="116" t="s">
+      <c r="H9" s="116" t="s">
+        <v>80</v>
+      </c>
+      <c r="I9" s="116" t="s">
+        <v>81</v>
+      </c>
+      <c r="J9" s="116" t="s">
         <v>69</v>
       </c>
-      <c r="K8" s="116" t="s">
-        <v>115</v>
-      </c>
-      <c r="L8" s="149" t="s">
-        <v>120</v>
-      </c>
-      <c r="M8" s="150"/>
-      <c r="N8" s="150"/>
-      <c r="O8" s="150"/>
-      <c r="P8" s="150"/>
-      <c r="Q8" s="117"/>
-      <c r="R8" s="117"/>
-      <c r="S8" s="117"/>
-      <c r="T8" s="117"/>
-      <c r="U8" s="118"/>
-      <c r="V8" s="116"/>
-      <c r="W8" s="119" t="s">
+      <c r="K9" s="116" t="s">
+        <v>113</v>
+      </c>
+      <c r="L9" s="147" t="s">
+        <v>118</v>
+      </c>
+      <c r="M9" s="148"/>
+      <c r="N9" s="148"/>
+      <c r="O9" s="148"/>
+      <c r="P9" s="148"/>
+      <c r="Q9" s="117"/>
+      <c r="R9" s="117"/>
+      <c r="S9" s="117"/>
+      <c r="T9" s="117"/>
+      <c r="U9" s="118"/>
+      <c r="V9" s="116"/>
+      <c r="W9" s="119" t="s">
         <v>64</v>
       </c>
-      <c r="X8" s="117"/>
-      <c r="Y8" s="117"/>
-      <c r="Z8" s="117"/>
-      <c r="AA8" s="117"/>
-      <c r="AB8" s="117"/>
-      <c r="AC8" s="117"/>
-      <c r="AD8" s="117"/>
-      <c r="AE8" s="117"/>
-      <c r="AF8" s="117"/>
-      <c r="AG8" s="117"/>
-      <c r="AH8" s="118"/>
-      <c r="AI8" s="26"/>
-    </row>
-    <row r="9" spans="1:51" s="18" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A9" s="26"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="30"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="28"/>
-      <c r="R9" s="28"/>
-      <c r="S9" s="28"/>
-      <c r="T9" s="28"/>
-      <c r="U9" s="28"/>
-      <c r="V9" s="21"/>
-      <c r="W9" s="31"/>
-      <c r="X9" s="28"/>
-      <c r="Y9" s="28"/>
-      <c r="Z9" s="28"/>
-      <c r="AA9" s="28"/>
-      <c r="AB9" s="28"/>
-      <c r="AC9" s="28"/>
-      <c r="AD9" s="28"/>
-      <c r="AE9" s="28"/>
-      <c r="AF9" s="28"/>
-      <c r="AG9" s="28"/>
-      <c r="AH9" s="28"/>
+      <c r="X9" s="117"/>
+      <c r="Y9" s="117"/>
+      <c r="Z9" s="117"/>
+      <c r="AA9" s="117"/>
+      <c r="AB9" s="117"/>
+      <c r="AC9" s="117"/>
+      <c r="AD9" s="117"/>
+      <c r="AE9" s="117"/>
+      <c r="AF9" s="117"/>
+      <c r="AG9" s="117"/>
+      <c r="AH9" s="118"/>
       <c r="AI9" s="26"/>
     </row>
-    <row r="10" spans="1:51" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
-      <c r="A10" s="35"/>
-      <c r="B10" s="47" t="s">
+    <row r="10" spans="1:51" s="18" customFormat="1" ht="24.95" customHeight="1">
+      <c r="A10" s="26"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="28"/>
+      <c r="R10" s="28"/>
+      <c r="S10" s="28"/>
+      <c r="T10" s="28"/>
+      <c r="U10" s="28"/>
+      <c r="V10" s="21"/>
+      <c r="W10" s="31"/>
+      <c r="X10" s="28"/>
+      <c r="Y10" s="28"/>
+      <c r="Z10" s="28"/>
+      <c r="AA10" s="28"/>
+      <c r="AB10" s="28"/>
+      <c r="AC10" s="28"/>
+      <c r="AD10" s="28"/>
+      <c r="AE10" s="28"/>
+      <c r="AF10" s="28"/>
+      <c r="AG10" s="28"/>
+      <c r="AH10" s="28"/>
+      <c r="AI10" s="26"/>
+    </row>
+    <row r="11" spans="1:51" s="10" customFormat="1" ht="39.950000000000003" customHeight="1">
+      <c r="A11" s="35"/>
+      <c r="B11" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="141" t="s">
-        <v>112</v>
-      </c>
-      <c r="D10" s="151"/>
-      <c r="E10" s="151"/>
-      <c r="F10" s="151"/>
-      <c r="G10" s="81" t="s">
+      <c r="C11" s="138" t="s">
+        <v>110</v>
+      </c>
+      <c r="D11" s="156"/>
+      <c r="E11" s="156"/>
+      <c r="F11" s="156"/>
+      <c r="G11" s="81" t="s">
+        <v>104</v>
+      </c>
+      <c r="H11" s="82" t="s">
+        <v>86</v>
+      </c>
+      <c r="I11" s="143" t="s">
+        <v>105</v>
+      </c>
+      <c r="J11" s="144"/>
+      <c r="K11" s="82" t="s">
+        <v>87</v>
+      </c>
+      <c r="L11" s="138" t="s">
         <v>106</v>
       </c>
-      <c r="H10" s="82" t="s">
-        <v>88</v>
-      </c>
-      <c r="I10" s="139" t="s">
+      <c r="M11" s="138"/>
+      <c r="N11" s="138"/>
+      <c r="O11" s="138"/>
+      <c r="P11" s="138" t="s">
         <v>107</v>
       </c>
-      <c r="J10" s="140"/>
-      <c r="K10" s="82" t="s">
-        <v>89</v>
-      </c>
-      <c r="L10" s="141" t="s">
+      <c r="Q11" s="138"/>
+      <c r="R11" s="138" t="s">
         <v>108</v>
       </c>
-      <c r="M10" s="141"/>
-      <c r="N10" s="141"/>
-      <c r="O10" s="141"/>
-      <c r="P10" s="141" t="s">
+      <c r="S11" s="138"/>
+      <c r="T11" s="138" t="s">
         <v>109</v>
       </c>
-      <c r="Q10" s="141"/>
-      <c r="R10" s="141" t="s">
-        <v>110</v>
-      </c>
-      <c r="S10" s="141"/>
-      <c r="T10" s="141" t="s">
-        <v>111</v>
-      </c>
-      <c r="U10" s="141"/>
-      <c r="V10" s="83"/>
-      <c r="W10" s="141" t="s">
-        <v>96</v>
-      </c>
-      <c r="X10" s="141"/>
-      <c r="Y10" s="141" t="s">
-        <v>99</v>
-      </c>
-      <c r="Z10" s="141"/>
-      <c r="AA10" s="141" t="s">
+      <c r="U11" s="138"/>
+      <c r="V11" s="83"/>
+      <c r="W11" s="138" t="s">
+        <v>94</v>
+      </c>
+      <c r="X11" s="138"/>
+      <c r="Y11" s="138" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z11" s="138"/>
+      <c r="AA11" s="138" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB11" s="138"/>
+      <c r="AC11" s="138" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD11" s="138"/>
+      <c r="AE11" s="138" t="s">
         <v>102</v>
       </c>
-      <c r="AB10" s="141"/>
-      <c r="AC10" s="141" t="s">
+      <c r="AF11" s="138"/>
+      <c r="AG11" s="138" t="s">
         <v>103</v>
       </c>
-      <c r="AD10" s="141"/>
-      <c r="AE10" s="141" t="s">
-        <v>104</v>
-      </c>
-      <c r="AF10" s="141"/>
-      <c r="AG10" s="141" t="s">
-        <v>105</v>
-      </c>
-      <c r="AH10" s="141"/>
-      <c r="AI10" s="42"/>
-      <c r="AJ10" s="9"/>
-      <c r="AK10" s="9"/>
-      <c r="AL10" s="9"/>
-      <c r="AM10" s="9"/>
-      <c r="AN10" s="9"/>
-      <c r="AO10" s="9"/>
-      <c r="AP10" s="9"/>
-      <c r="AQ10" s="9"/>
-      <c r="AR10" s="9"/>
-      <c r="AS10" s="9"/>
-      <c r="AT10" s="9"/>
-      <c r="AU10" s="9"/>
-      <c r="AV10" s="9"/>
-      <c r="AW10" s="9"/>
-      <c r="AX10" s="9"/>
-      <c r="AY10" s="9"/>
+      <c r="AH11" s="138"/>
+      <c r="AI11" s="42"/>
+      <c r="AJ11" s="9"/>
+      <c r="AK11" s="9"/>
+      <c r="AL11" s="9"/>
+      <c r="AM11" s="9"/>
+      <c r="AN11" s="9"/>
+      <c r="AO11" s="9"/>
+      <c r="AP11" s="9"/>
+      <c r="AQ11" s="9"/>
+      <c r="AR11" s="9"/>
+      <c r="AS11" s="9"/>
+      <c r="AT11" s="9"/>
+      <c r="AU11" s="9"/>
+      <c r="AV11" s="9"/>
+      <c r="AW11" s="9"/>
+      <c r="AX11" s="9"/>
+      <c r="AY11" s="9"/>
     </row>
-    <row r="11" spans="1:51" s="5" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A11" s="36"/>
-      <c r="B11" s="48" t="s">
+    <row r="12" spans="1:51" s="5" customFormat="1" ht="24.95" customHeight="1">
+      <c r="A12" s="36"/>
+      <c r="B12" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="84"/>
-      <c r="D11" s="85"/>
-      <c r="E11" s="85"/>
-      <c r="F11" s="86"/>
-      <c r="G11" s="87"/>
-      <c r="H11" s="88"/>
-      <c r="I11" s="89"/>
-      <c r="J11" s="90"/>
-      <c r="K11" s="89"/>
-      <c r="L11" s="89"/>
-      <c r="M11" s="89"/>
-      <c r="N11" s="91"/>
-      <c r="O11" s="89"/>
-      <c r="P11" s="89"/>
-      <c r="Q11" s="89"/>
-      <c r="R11" s="89"/>
-      <c r="S11" s="89"/>
-      <c r="T11" s="89"/>
-      <c r="U11" s="89"/>
-      <c r="V11" s="90"/>
-      <c r="W11" s="89"/>
-      <c r="X11" s="89"/>
-      <c r="Y11" s="89"/>
-      <c r="Z11" s="89"/>
-      <c r="AA11" s="89"/>
-      <c r="AB11" s="89"/>
-      <c r="AC11" s="89"/>
-      <c r="AD11" s="89"/>
-      <c r="AE11" s="89"/>
-      <c r="AF11" s="89"/>
-      <c r="AG11" s="89"/>
-      <c r="AH11" s="92"/>
-      <c r="AI11" s="43"/>
-      <c r="AJ11" s="11"/>
-      <c r="AK11" s="11"/>
-      <c r="AL11" s="11"/>
-      <c r="AM11" s="11"/>
-      <c r="AN11" s="11"/>
-      <c r="AO11" s="11"/>
-      <c r="AP11" s="11"/>
-      <c r="AQ11" s="11"/>
-      <c r="AR11" s="11"/>
-      <c r="AS11" s="11"/>
-      <c r="AT11" s="11"/>
-      <c r="AU11" s="11"/>
-      <c r="AV11" s="11"/>
-      <c r="AW11" s="11"/>
-      <c r="AX11" s="11"/>
-      <c r="AY11" s="11"/>
-    </row>
-    <row r="12" spans="1:51" s="5" customFormat="1" ht="51" customHeight="1">
-      <c r="A12" s="36"/>
-      <c r="B12" s="47" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" s="145"/>
-      <c r="D12" s="145"/>
-      <c r="E12" s="145"/>
-      <c r="F12" s="145"/>
-      <c r="G12" s="93"/>
-      <c r="H12" s="94"/>
-      <c r="I12" s="82" t="s">
-        <v>77</v>
-      </c>
-      <c r="J12" s="82" t="s">
-        <v>78</v>
-      </c>
-      <c r="K12" s="94"/>
-      <c r="L12" s="88" t="s">
-        <v>90</v>
-      </c>
-      <c r="M12" s="88" t="s">
-        <v>91</v>
-      </c>
-      <c r="N12" s="88" t="s">
-        <v>92</v>
-      </c>
-      <c r="O12" s="88" t="s">
-        <v>93</v>
-      </c>
-      <c r="P12" s="88" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q12" s="88" t="s">
-        <v>95</v>
-      </c>
-      <c r="R12" s="88" t="s">
-        <v>39</v>
-      </c>
-      <c r="S12" s="88" t="s">
-        <v>40</v>
-      </c>
-      <c r="T12" s="88" t="s">
-        <v>41</v>
-      </c>
-      <c r="U12" s="88" t="s">
-        <v>42</v>
-      </c>
-      <c r="V12" s="94"/>
-      <c r="W12" s="88" t="s">
-        <v>97</v>
-      </c>
-      <c r="X12" s="88" t="s">
-        <v>98</v>
-      </c>
-      <c r="Y12" s="88" t="s">
-        <v>100</v>
-      </c>
-      <c r="Z12" s="88" t="s">
-        <v>101</v>
-      </c>
-      <c r="AA12" s="88" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB12" s="88" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC12" s="88" t="s">
-        <v>45</v>
-      </c>
-      <c r="AD12" s="88" t="s">
-        <v>46</v>
-      </c>
-      <c r="AE12" s="88" t="s">
-        <v>47</v>
-      </c>
-      <c r="AF12" s="88" t="s">
-        <v>48</v>
-      </c>
-      <c r="AG12" s="88" t="s">
-        <v>49</v>
-      </c>
-      <c r="AH12" s="88" t="s">
-        <v>50</v>
-      </c>
+      <c r="C12" s="84"/>
+      <c r="D12" s="85"/>
+      <c r="E12" s="85"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="87"/>
+      <c r="H12" s="88"/>
+      <c r="I12" s="89"/>
+      <c r="J12" s="90"/>
+      <c r="K12" s="89"/>
+      <c r="L12" s="89"/>
+      <c r="M12" s="89"/>
+      <c r="N12" s="91"/>
+      <c r="O12" s="89"/>
+      <c r="P12" s="89"/>
+      <c r="Q12" s="89"/>
+      <c r="R12" s="89"/>
+      <c r="S12" s="89"/>
+      <c r="T12" s="89"/>
+      <c r="U12" s="89"/>
+      <c r="V12" s="90"/>
+      <c r="W12" s="89"/>
+      <c r="X12" s="89"/>
+      <c r="Y12" s="89"/>
+      <c r="Z12" s="89"/>
+      <c r="AA12" s="89"/>
+      <c r="AB12" s="89"/>
+      <c r="AC12" s="89"/>
+      <c r="AD12" s="89"/>
+      <c r="AE12" s="89"/>
+      <c r="AF12" s="89"/>
+      <c r="AG12" s="89"/>
+      <c r="AH12" s="92"/>
       <c r="AI12" s="43"/>
       <c r="AJ12" s="11"/>
       <c r="AK12" s="11"/>
@@ -2766,43 +2663,91 @@
       <c r="AX12" s="11"/>
       <c r="AY12" s="11"/>
     </row>
-    <row r="13" spans="1:51" s="5" customFormat="1" ht="24.95" customHeight="1">
+    <row r="13" spans="1:51" s="5" customFormat="1" ht="51" customHeight="1">
       <c r="A13" s="36"/>
-      <c r="B13" s="48" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="85"/>
-      <c r="D13" s="85"/>
-      <c r="E13" s="85"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="85"/>
-      <c r="H13" s="95"/>
-      <c r="I13" s="89"/>
-      <c r="J13" s="89"/>
-      <c r="K13" s="90"/>
-      <c r="L13" s="89"/>
-      <c r="M13" s="89"/>
-      <c r="N13" s="91"/>
-      <c r="O13" s="89"/>
-      <c r="P13" s="89"/>
-      <c r="Q13" s="89"/>
-      <c r="R13" s="89"/>
-      <c r="S13" s="89"/>
-      <c r="T13" s="89"/>
-      <c r="U13" s="89"/>
-      <c r="V13" s="90"/>
-      <c r="W13" s="89"/>
-      <c r="X13" s="89"/>
-      <c r="Y13" s="89"/>
-      <c r="Z13" s="89"/>
-      <c r="AA13" s="89"/>
-      <c r="AB13" s="89"/>
-      <c r="AC13" s="89"/>
-      <c r="AD13" s="89"/>
-      <c r="AE13" s="89"/>
-      <c r="AF13" s="89"/>
-      <c r="AG13" s="89"/>
-      <c r="AH13" s="92"/>
+      <c r="B13" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="157"/>
+      <c r="D13" s="157"/>
+      <c r="E13" s="157"/>
+      <c r="F13" s="157"/>
+      <c r="G13" s="93"/>
+      <c r="H13" s="94"/>
+      <c r="I13" s="82" t="s">
+        <v>160</v>
+      </c>
+      <c r="J13" s="82" t="s">
+        <v>161</v>
+      </c>
+      <c r="K13" s="94"/>
+      <c r="L13" s="88" t="s">
+        <v>88</v>
+      </c>
+      <c r="M13" s="88" t="s">
+        <v>89</v>
+      </c>
+      <c r="N13" s="88" t="s">
+        <v>90</v>
+      </c>
+      <c r="O13" s="88" t="s">
+        <v>91</v>
+      </c>
+      <c r="P13" s="88" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q13" s="88" t="s">
+        <v>93</v>
+      </c>
+      <c r="R13" s="88" t="s">
+        <v>39</v>
+      </c>
+      <c r="S13" s="88" t="s">
+        <v>40</v>
+      </c>
+      <c r="T13" s="88" t="s">
+        <v>41</v>
+      </c>
+      <c r="U13" s="88" t="s">
+        <v>42</v>
+      </c>
+      <c r="V13" s="94"/>
+      <c r="W13" s="88" t="s">
+        <v>95</v>
+      </c>
+      <c r="X13" s="88" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y13" s="88" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z13" s="88" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA13" s="88" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB13" s="88" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC13" s="88" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD13" s="88" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE13" s="88" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF13" s="88" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG13" s="88" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH13" s="88" t="s">
+        <v>50</v>
+      </c>
       <c r="AI13" s="43"/>
       <c r="AJ13" s="11"/>
       <c r="AK13" s="11"/>
@@ -2821,505 +2766,523 @@
       <c r="AX13" s="11"/>
       <c r="AY13" s="11"/>
     </row>
-    <row r="14" spans="1:51" s="8" customFormat="1" ht="25.5">
-      <c r="A14" s="37"/>
-      <c r="B14" s="96" t="s">
+    <row r="14" spans="1:51" s="5" customFormat="1" ht="24.95" customHeight="1">
+      <c r="A14" s="36"/>
+      <c r="B14" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="85"/>
+      <c r="D14" s="85"/>
+      <c r="E14" s="85"/>
+      <c r="F14" s="86"/>
+      <c r="G14" s="85"/>
+      <c r="H14" s="95"/>
+      <c r="I14" s="89"/>
+      <c r="J14" s="89"/>
+      <c r="K14" s="90"/>
+      <c r="L14" s="89"/>
+      <c r="M14" s="89"/>
+      <c r="N14" s="91"/>
+      <c r="O14" s="89"/>
+      <c r="P14" s="89"/>
+      <c r="Q14" s="89"/>
+      <c r="R14" s="89"/>
+      <c r="S14" s="89"/>
+      <c r="T14" s="89"/>
+      <c r="U14" s="89"/>
+      <c r="V14" s="90"/>
+      <c r="W14" s="89"/>
+      <c r="X14" s="89"/>
+      <c r="Y14" s="89"/>
+      <c r="Z14" s="89"/>
+      <c r="AA14" s="89"/>
+      <c r="AB14" s="89"/>
+      <c r="AC14" s="89"/>
+      <c r="AD14" s="89"/>
+      <c r="AE14" s="89"/>
+      <c r="AF14" s="89"/>
+      <c r="AG14" s="89"/>
+      <c r="AH14" s="92"/>
+      <c r="AI14" s="43"/>
+      <c r="AJ14" s="11"/>
+      <c r="AK14" s="11"/>
+      <c r="AL14" s="11"/>
+      <c r="AM14" s="11"/>
+      <c r="AN14" s="11"/>
+      <c r="AO14" s="11"/>
+      <c r="AP14" s="11"/>
+      <c r="AQ14" s="11"/>
+      <c r="AR14" s="11"/>
+      <c r="AS14" s="11"/>
+      <c r="AT14" s="11"/>
+      <c r="AU14" s="11"/>
+      <c r="AV14" s="11"/>
+      <c r="AW14" s="11"/>
+      <c r="AX14" s="11"/>
+      <c r="AY14" s="11"/>
+    </row>
+    <row r="15" spans="1:51" s="8" customFormat="1" ht="25.5">
+      <c r="A15" s="37"/>
+      <c r="B15" s="96" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="138" t="s">
+      <c r="C15" s="142" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="138"/>
-      <c r="E14" s="138"/>
-      <c r="F14" s="138"/>
-      <c r="G14" s="96" t="s">
+      <c r="D15" s="142"/>
+      <c r="E15" s="142"/>
+      <c r="F15" s="142"/>
+      <c r="G15" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="H14" s="96" t="s">
+      <c r="H15" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="I14" s="97" t="s">
+      <c r="I15" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="J14" s="96" t="s">
+      <c r="J15" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="K14" s="96" t="s">
+      <c r="K15" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="L14" s="138" t="s">
+      <c r="L15" s="142" t="s">
         <v>5</v>
       </c>
-      <c r="M14" s="138"/>
-      <c r="N14" s="138"/>
-      <c r="O14" s="138"/>
-      <c r="P14" s="138" t="s">
+      <c r="M15" s="142"/>
+      <c r="N15" s="142"/>
+      <c r="O15" s="142"/>
+      <c r="P15" s="142" t="s">
         <v>5</v>
       </c>
-      <c r="Q14" s="138"/>
-      <c r="R14" s="138" t="s">
+      <c r="Q15" s="142"/>
+      <c r="R15" s="142" t="s">
         <v>6</v>
       </c>
-      <c r="S14" s="138"/>
-      <c r="T14" s="138" t="s">
+      <c r="S15" s="142"/>
+      <c r="T15" s="142" t="s">
         <v>7</v>
       </c>
-      <c r="U14" s="138"/>
-      <c r="V14" s="98"/>
-      <c r="W14" s="138" t="s">
+      <c r="U15" s="142"/>
+      <c r="V15" s="98"/>
+      <c r="W15" s="142" t="s">
         <v>8</v>
       </c>
-      <c r="X14" s="138"/>
-      <c r="Y14" s="138" t="s">
+      <c r="X15" s="142"/>
+      <c r="Y15" s="142" t="s">
         <v>8</v>
       </c>
-      <c r="Z14" s="138"/>
-      <c r="AA14" s="138" t="s">
+      <c r="Z15" s="142"/>
+      <c r="AA15" s="142" t="s">
         <v>8</v>
       </c>
-      <c r="AB14" s="138"/>
-      <c r="AC14" s="138" t="s">
+      <c r="AB15" s="142"/>
+      <c r="AC15" s="142" t="s">
         <v>8</v>
       </c>
-      <c r="AD14" s="138"/>
-      <c r="AE14" s="138" t="s">
+      <c r="AD15" s="142"/>
+      <c r="AE15" s="142" t="s">
         <v>8</v>
       </c>
-      <c r="AF14" s="138"/>
-      <c r="AG14" s="138" t="s">
+      <c r="AF15" s="142"/>
+      <c r="AG15" s="142" t="s">
         <v>8</v>
       </c>
-      <c r="AH14" s="138"/>
-      <c r="AI14" s="41"/>
-      <c r="AJ14" s="7"/>
-      <c r="AK14" s="7"/>
-      <c r="AL14" s="7"/>
-      <c r="AM14" s="7"/>
-      <c r="AN14" s="7"/>
-      <c r="AO14" s="7"/>
-      <c r="AP14" s="7"/>
-      <c r="AQ14" s="7"/>
-      <c r="AR14" s="7"/>
-      <c r="AS14" s="7"/>
-      <c r="AT14" s="7"/>
-      <c r="AU14" s="7"/>
-      <c r="AV14" s="7"/>
-      <c r="AW14" s="7"/>
-      <c r="AX14" s="7"/>
-      <c r="AY14" s="7"/>
+      <c r="AH15" s="142"/>
+      <c r="AI15" s="41"/>
+      <c r="AJ15" s="7"/>
+      <c r="AK15" s="7"/>
+      <c r="AL15" s="7"/>
+      <c r="AM15" s="7"/>
+      <c r="AN15" s="7"/>
+      <c r="AO15" s="7"/>
+      <c r="AP15" s="7"/>
+      <c r="AQ15" s="7"/>
+      <c r="AR15" s="7"/>
+      <c r="AS15" s="7"/>
+      <c r="AT15" s="7"/>
+      <c r="AU15" s="7"/>
+      <c r="AV15" s="7"/>
+      <c r="AW15" s="7"/>
+      <c r="AX15" s="7"/>
+      <c r="AY15" s="7"/>
     </row>
-    <row r="15" spans="1:51" ht="24" customHeight="1">
-      <c r="A15" s="19"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="21"/>
-      <c r="N15" s="21"/>
-      <c r="O15" s="21"/>
-      <c r="P15" s="21"/>
-      <c r="Q15" s="21"/>
-      <c r="R15" s="21"/>
-      <c r="S15" s="21"/>
-      <c r="T15" s="21"/>
-      <c r="U15" s="21"/>
-      <c r="V15" s="21"/>
-      <c r="W15" s="21"/>
-      <c r="X15" s="21"/>
-      <c r="Y15" s="21"/>
-      <c r="Z15" s="21"/>
-      <c r="AA15" s="21"/>
-      <c r="AB15" s="21"/>
-      <c r="AC15" s="21"/>
-      <c r="AD15" s="21"/>
-      <c r="AE15" s="21"/>
-      <c r="AF15" s="21"/>
-      <c r="AG15" s="21"/>
-      <c r="AH15" s="21"/>
-      <c r="AI15" s="21"/>
-    </row>
-    <row r="16" spans="1:51" ht="51" customHeight="1">
+    <row r="16" spans="1:51" ht="24" customHeight="1">
       <c r="A16" s="19"/>
-      <c r="B16" s="49" t="s">
-        <v>118</v>
-      </c>
-      <c r="C16" s="52" t="s">
-        <v>121</v>
-      </c>
-      <c r="D16" s="53" t="s">
-        <v>151</v>
-      </c>
-      <c r="E16" s="54"/>
-      <c r="F16" s="54"/>
-      <c r="G16" s="55" t="s">
-        <v>122</v>
-      </c>
-      <c r="H16" s="54"/>
-      <c r="I16" s="54"/>
-      <c r="J16" s="54"/>
-      <c r="K16" s="53" t="s">
-        <v>123</v>
-      </c>
-      <c r="L16" s="154" t="s">
-        <v>152</v>
-      </c>
-      <c r="M16" s="154"/>
-      <c r="N16" s="154"/>
-      <c r="O16" s="154"/>
-      <c r="P16" s="154" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q16" s="154"/>
-      <c r="R16" s="154" t="s">
-        <v>154</v>
-      </c>
-      <c r="S16" s="154"/>
-      <c r="T16" s="154" t="s">
-        <v>155</v>
-      </c>
-      <c r="U16" s="154"/>
-      <c r="V16" s="53" t="s">
-        <v>132</v>
-      </c>
-      <c r="W16" s="154" t="s">
-        <v>133</v>
-      </c>
-      <c r="X16" s="154"/>
-      <c r="Y16" s="154" t="s">
-        <v>136</v>
-      </c>
-      <c r="Z16" s="154"/>
-      <c r="AA16" s="154" t="s">
-        <v>139</v>
-      </c>
-      <c r="AB16" s="154"/>
-      <c r="AC16" s="154" t="s">
-        <v>142</v>
-      </c>
-      <c r="AD16" s="154"/>
-      <c r="AE16" s="154" t="s">
-        <v>145</v>
-      </c>
-      <c r="AF16" s="154"/>
-      <c r="AG16" s="154" t="s">
-        <v>148</v>
-      </c>
-      <c r="AH16" s="154"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="21"/>
+      <c r="O16" s="21"/>
+      <c r="P16" s="21"/>
+      <c r="Q16" s="21"/>
+      <c r="R16" s="21"/>
+      <c r="S16" s="21"/>
+      <c r="T16" s="21"/>
+      <c r="U16" s="21"/>
+      <c r="V16" s="21"/>
+      <c r="W16" s="21"/>
+      <c r="X16" s="21"/>
+      <c r="Y16" s="21"/>
+      <c r="Z16" s="21"/>
+      <c r="AA16" s="21"/>
+      <c r="AB16" s="21"/>
+      <c r="AC16" s="21"/>
+      <c r="AD16" s="21"/>
+      <c r="AE16" s="21"/>
+      <c r="AF16" s="21"/>
+      <c r="AG16" s="21"/>
+      <c r="AH16" s="21"/>
       <c r="AI16" s="21"/>
     </row>
-    <row r="17" spans="1:35" ht="27.75" customHeight="1">
+    <row r="17" spans="1:35" ht="51" customHeight="1">
       <c r="A17" s="19"/>
-      <c r="B17" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" s="56"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="58"/>
-      <c r="F17" s="58"/>
-      <c r="G17" s="59"/>
-      <c r="H17" s="60"/>
-      <c r="I17" s="60"/>
-      <c r="J17" s="60"/>
-      <c r="K17" s="49"/>
-      <c r="L17" s="61"/>
-      <c r="M17" s="62"/>
-      <c r="N17" s="63"/>
-      <c r="O17" s="62"/>
-      <c r="P17" s="61"/>
-      <c r="Q17" s="62"/>
-      <c r="R17" s="61"/>
-      <c r="S17" s="62"/>
-      <c r="T17" s="61"/>
-      <c r="U17" s="62"/>
-      <c r="V17" s="49"/>
-      <c r="W17" s="61"/>
-      <c r="X17" s="62"/>
-      <c r="Y17" s="61"/>
-      <c r="Z17" s="62"/>
-      <c r="AA17" s="61"/>
-      <c r="AB17" s="62"/>
-      <c r="AC17" s="61"/>
-      <c r="AD17" s="62"/>
-      <c r="AE17" s="61"/>
-      <c r="AF17" s="62"/>
-      <c r="AG17" s="61"/>
-      <c r="AH17" s="63"/>
+      <c r="B17" s="49" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="D17" s="53" t="s">
+        <v>149</v>
+      </c>
+      <c r="E17" s="54"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="55" t="s">
+        <v>120</v>
+      </c>
+      <c r="H17" s="54"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="54"/>
+      <c r="K17" s="53" t="s">
+        <v>121</v>
+      </c>
+      <c r="L17" s="145" t="s">
+        <v>150</v>
+      </c>
+      <c r="M17" s="145"/>
+      <c r="N17" s="145"/>
+      <c r="O17" s="145"/>
+      <c r="P17" s="145" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q17" s="145"/>
+      <c r="R17" s="145" t="s">
+        <v>152</v>
+      </c>
+      <c r="S17" s="145"/>
+      <c r="T17" s="145" t="s">
+        <v>153</v>
+      </c>
+      <c r="U17" s="145"/>
+      <c r="V17" s="53" t="s">
+        <v>130</v>
+      </c>
+      <c r="W17" s="145" t="s">
+        <v>131</v>
+      </c>
+      <c r="X17" s="145"/>
+      <c r="Y17" s="145" t="s">
+        <v>134</v>
+      </c>
+      <c r="Z17" s="145"/>
+      <c r="AA17" s="145" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB17" s="145"/>
+      <c r="AC17" s="145" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD17" s="145"/>
+      <c r="AE17" s="145" t="s">
+        <v>143</v>
+      </c>
+      <c r="AF17" s="145"/>
+      <c r="AG17" s="145" t="s">
+        <v>146</v>
+      </c>
+      <c r="AH17" s="145"/>
       <c r="AI17" s="21"/>
     </row>
-    <row r="18" spans="1:35" ht="48" customHeight="1">
+    <row r="18" spans="1:35" ht="27.75" customHeight="1">
       <c r="A18" s="19"/>
-      <c r="B18" s="49" t="s">
-        <v>118</v>
-      </c>
-      <c r="C18" s="64"/>
-      <c r="D18" s="54"/>
+      <c r="B18" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="56"/>
+      <c r="D18" s="57"/>
       <c r="E18" s="58"/>
       <c r="F18" s="58"/>
-      <c r="G18" s="58"/>
-      <c r="H18" s="65"/>
-      <c r="I18" s="66"/>
-      <c r="J18" s="66"/>
-      <c r="K18" s="65"/>
-      <c r="L18" s="67" t="s">
-        <v>124</v>
-      </c>
-      <c r="M18" s="68" t="s">
-        <v>125</v>
-      </c>
-      <c r="N18" s="69"/>
-      <c r="O18" s="69"/>
-      <c r="P18" s="67" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q18" s="68" t="s">
-        <v>127</v>
-      </c>
-      <c r="R18" s="67" t="s">
-        <v>128</v>
-      </c>
-      <c r="S18" s="68" t="s">
-        <v>129</v>
-      </c>
-      <c r="T18" s="67" t="s">
-        <v>130</v>
-      </c>
-      <c r="U18" s="68" t="s">
-        <v>131</v>
-      </c>
-      <c r="V18" s="65"/>
-      <c r="W18" s="67" t="s">
-        <v>134</v>
-      </c>
-      <c r="X18" s="67" t="s">
-        <v>135</v>
-      </c>
-      <c r="Y18" s="67" t="s">
-        <v>137</v>
-      </c>
-      <c r="Z18" s="67" t="s">
-        <v>138</v>
-      </c>
-      <c r="AA18" s="67" t="s">
-        <v>140</v>
-      </c>
-      <c r="AB18" s="67" t="s">
-        <v>141</v>
-      </c>
-      <c r="AC18" s="67" t="s">
-        <v>143</v>
-      </c>
-      <c r="AD18" s="67" t="s">
-        <v>144</v>
-      </c>
-      <c r="AE18" s="67" t="s">
-        <v>146</v>
-      </c>
-      <c r="AF18" s="67" t="s">
-        <v>147</v>
-      </c>
-      <c r="AG18" s="67" t="s">
-        <v>149</v>
-      </c>
-      <c r="AH18" s="70" t="s">
-        <v>150</v>
-      </c>
+      <c r="G18" s="59"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="49"/>
+      <c r="L18" s="61"/>
+      <c r="M18" s="62"/>
+      <c r="N18" s="63"/>
+      <c r="O18" s="62"/>
+      <c r="P18" s="61"/>
+      <c r="Q18" s="62"/>
+      <c r="R18" s="61"/>
+      <c r="S18" s="62"/>
+      <c r="T18" s="61"/>
+      <c r="U18" s="62"/>
+      <c r="V18" s="49"/>
+      <c r="W18" s="61"/>
+      <c r="X18" s="62"/>
+      <c r="Y18" s="61"/>
+      <c r="Z18" s="62"/>
+      <c r="AA18" s="61"/>
+      <c r="AB18" s="62"/>
+      <c r="AC18" s="61"/>
+      <c r="AD18" s="62"/>
+      <c r="AE18" s="61"/>
+      <c r="AF18" s="62"/>
+      <c r="AG18" s="61"/>
+      <c r="AH18" s="63"/>
       <c r="AI18" s="21"/>
     </row>
-    <row r="19" spans="1:35" ht="27.75" customHeight="1">
+    <row r="19" spans="1:35" ht="48" customHeight="1">
       <c r="A19" s="19"/>
-      <c r="B19" s="50" t="s">
-        <v>63</v>
+      <c r="B19" s="49" t="s">
+        <v>116</v>
       </c>
       <c r="C19" s="64"/>
       <c r="D19" s="54"/>
       <c r="E19" s="58"/>
       <c r="F19" s="58"/>
       <c r="G19" s="58"/>
-      <c r="H19" s="60"/>
-      <c r="I19" s="60"/>
-      <c r="J19" s="60"/>
-      <c r="K19" s="60"/>
-      <c r="L19" s="70"/>
-      <c r="M19" s="70"/>
-      <c r="N19" s="63"/>
-      <c r="O19" s="63"/>
-      <c r="P19" s="70"/>
-      <c r="Q19" s="70"/>
-      <c r="R19" s="70"/>
-      <c r="S19" s="70"/>
-      <c r="T19" s="70"/>
-      <c r="U19" s="70"/>
-      <c r="V19" s="60"/>
-      <c r="W19" s="70"/>
-      <c r="X19" s="70"/>
-      <c r="Y19" s="70"/>
-      <c r="Z19" s="70"/>
-      <c r="AA19" s="70"/>
-      <c r="AB19" s="70"/>
-      <c r="AC19" s="70"/>
-      <c r="AD19" s="70"/>
-      <c r="AE19" s="70"/>
-      <c r="AF19" s="70"/>
-      <c r="AG19" s="70"/>
-      <c r="AH19" s="70"/>
+      <c r="H19" s="65"/>
+      <c r="I19" s="66"/>
+      <c r="J19" s="66"/>
+      <c r="K19" s="65"/>
+      <c r="L19" s="67" t="s">
+        <v>122</v>
+      </c>
+      <c r="M19" s="68" t="s">
+        <v>123</v>
+      </c>
+      <c r="N19" s="69"/>
+      <c r="O19" s="69"/>
+      <c r="P19" s="67" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q19" s="68" t="s">
+        <v>125</v>
+      </c>
+      <c r="R19" s="67" t="s">
+        <v>126</v>
+      </c>
+      <c r="S19" s="68" t="s">
+        <v>127</v>
+      </c>
+      <c r="T19" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="U19" s="68" t="s">
+        <v>129</v>
+      </c>
+      <c r="V19" s="65"/>
+      <c r="W19" s="67" t="s">
+        <v>132</v>
+      </c>
+      <c r="X19" s="67" t="s">
+        <v>133</v>
+      </c>
+      <c r="Y19" s="67" t="s">
+        <v>135</v>
+      </c>
+      <c r="Z19" s="67" t="s">
+        <v>136</v>
+      </c>
+      <c r="AA19" s="67" t="s">
+        <v>138</v>
+      </c>
+      <c r="AB19" s="67" t="s">
+        <v>139</v>
+      </c>
+      <c r="AC19" s="67" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD19" s="67" t="s">
+        <v>142</v>
+      </c>
+      <c r="AE19" s="67" t="s">
+        <v>144</v>
+      </c>
+      <c r="AF19" s="67" t="s">
+        <v>145</v>
+      </c>
+      <c r="AG19" s="67" t="s">
+        <v>147</v>
+      </c>
+      <c r="AH19" s="70" t="s">
+        <v>148</v>
+      </c>
       <c r="AI19" s="21"/>
     </row>
-    <row r="20" spans="1:35" ht="24" customHeight="1">
+    <row r="20" spans="1:35" ht="27.75" customHeight="1">
       <c r="A20" s="19"/>
-      <c r="B20" s="71" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="72" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" s="72" t="s">
-        <v>5</v>
-      </c>
+      <c r="B20" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="64"/>
+      <c r="D20" s="54"/>
       <c r="E20" s="58"/>
       <c r="F20" s="58"/>
-      <c r="G20" s="73" t="s">
-        <v>5</v>
-      </c>
-      <c r="H20" s="74"/>
-      <c r="I20" s="74"/>
-      <c r="J20" s="74"/>
-      <c r="K20" s="71" t="s">
-        <v>5</v>
-      </c>
-      <c r="L20" s="157" t="s">
-        <v>5</v>
-      </c>
-      <c r="M20" s="157"/>
-      <c r="N20" s="157"/>
-      <c r="O20" s="157"/>
-      <c r="P20" s="157" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q20" s="157"/>
-      <c r="R20" s="157" t="s">
-        <v>6</v>
-      </c>
-      <c r="S20" s="157"/>
-      <c r="T20" s="157" t="s">
-        <v>7</v>
-      </c>
-      <c r="U20" s="157"/>
-      <c r="V20" s="75" t="s">
-        <v>5</v>
-      </c>
-      <c r="W20" s="157" t="s">
-        <v>8</v>
-      </c>
-      <c r="X20" s="157"/>
-      <c r="Y20" s="157" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z20" s="157"/>
-      <c r="AA20" s="157" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB20" s="157"/>
-      <c r="AC20" s="157" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD20" s="157"/>
-      <c r="AE20" s="157" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF20" s="157"/>
-      <c r="AG20" s="157" t="s">
-        <v>8</v>
-      </c>
-      <c r="AH20" s="157"/>
+      <c r="G20" s="58"/>
+      <c r="H20" s="60"/>
+      <c r="I20" s="60"/>
+      <c r="J20" s="60"/>
+      <c r="K20" s="60"/>
+      <c r="L20" s="70"/>
+      <c r="M20" s="70"/>
+      <c r="N20" s="63"/>
+      <c r="O20" s="63"/>
+      <c r="P20" s="70"/>
+      <c r="Q20" s="70"/>
+      <c r="R20" s="70"/>
+      <c r="S20" s="70"/>
+      <c r="T20" s="70"/>
+      <c r="U20" s="70"/>
+      <c r="V20" s="60"/>
+      <c r="W20" s="70"/>
+      <c r="X20" s="70"/>
+      <c r="Y20" s="70"/>
+      <c r="Z20" s="70"/>
+      <c r="AA20" s="70"/>
+      <c r="AB20" s="70"/>
+      <c r="AC20" s="70"/>
+      <c r="AD20" s="70"/>
+      <c r="AE20" s="70"/>
+      <c r="AF20" s="70"/>
+      <c r="AG20" s="70"/>
+      <c r="AH20" s="70"/>
       <c r="AI20" s="21"/>
     </row>
-    <row r="21" spans="1:35" ht="54" customHeight="1">
+    <row r="21" spans="1:35" ht="24" customHeight="1">
       <c r="A21" s="19"/>
-      <c r="B21" s="76" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="64"/>
-      <c r="D21" s="54"/>
+      <c r="B21" s="71" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="72" t="s">
+        <v>5</v>
+      </c>
       <c r="E21" s="58"/>
       <c r="F21" s="58"/>
-      <c r="G21" s="58"/>
-      <c r="H21" s="77"/>
-      <c r="I21" s="77"/>
-      <c r="J21" s="77"/>
-      <c r="K21" s="77" t="s">
-        <v>115</v>
-      </c>
-      <c r="L21" s="155" t="s">
-        <v>119</v>
-      </c>
-      <c r="M21" s="156"/>
-      <c r="N21" s="156"/>
-      <c r="O21" s="156"/>
-      <c r="P21" s="156"/>
-      <c r="Q21" s="78"/>
-      <c r="R21" s="78"/>
-      <c r="S21" s="78"/>
-      <c r="T21" s="78"/>
-      <c r="U21" s="79"/>
-      <c r="V21" s="77"/>
-      <c r="W21" s="80" t="s">
-        <v>64</v>
-      </c>
-      <c r="X21" s="78"/>
-      <c r="Y21" s="78"/>
-      <c r="Z21" s="78"/>
-      <c r="AA21" s="78"/>
-      <c r="AB21" s="78"/>
-      <c r="AC21" s="78"/>
-      <c r="AD21" s="78"/>
-      <c r="AE21" s="78"/>
-      <c r="AF21" s="78"/>
-      <c r="AG21" s="78"/>
-      <c r="AH21" s="79"/>
+      <c r="G21" s="73" t="s">
+        <v>5</v>
+      </c>
+      <c r="H21" s="74"/>
+      <c r="I21" s="74"/>
+      <c r="J21" s="74"/>
+      <c r="K21" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="L21" s="146" t="s">
+        <v>5</v>
+      </c>
+      <c r="M21" s="146"/>
+      <c r="N21" s="146"/>
+      <c r="O21" s="146"/>
+      <c r="P21" s="146" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q21" s="146"/>
+      <c r="R21" s="146" t="s">
+        <v>6</v>
+      </c>
+      <c r="S21" s="146"/>
+      <c r="T21" s="146" t="s">
+        <v>7</v>
+      </c>
+      <c r="U21" s="146"/>
+      <c r="V21" s="75" t="s">
+        <v>5</v>
+      </c>
+      <c r="W21" s="146" t="s">
+        <v>8</v>
+      </c>
+      <c r="X21" s="146"/>
+      <c r="Y21" s="146" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z21" s="146"/>
+      <c r="AA21" s="146" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB21" s="146"/>
+      <c r="AC21" s="146" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD21" s="146"/>
+      <c r="AE21" s="146" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF21" s="146"/>
+      <c r="AG21" s="146" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH21" s="146"/>
       <c r="AI21" s="21"/>
     </row>
-    <row r="22" spans="1:35" ht="24" customHeight="1">
+    <row r="22" spans="1:35" ht="54" customHeight="1">
       <c r="A22" s="19"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="21"/>
-      <c r="N22" s="21"/>
-      <c r="O22" s="21"/>
-      <c r="P22" s="21"/>
-      <c r="Q22" s="21"/>
-      <c r="R22" s="21"/>
-      <c r="S22" s="21"/>
-      <c r="T22" s="21"/>
-      <c r="U22" s="21"/>
-      <c r="V22" s="21"/>
-      <c r="W22" s="21"/>
-      <c r="X22" s="21"/>
-      <c r="Y22" s="21"/>
-      <c r="Z22" s="21"/>
-      <c r="AA22" s="21"/>
-      <c r="AB22" s="21"/>
-      <c r="AC22" s="21"/>
-      <c r="AD22" s="21"/>
-      <c r="AE22" s="21"/>
-      <c r="AF22" s="21"/>
-      <c r="AG22" s="21"/>
-      <c r="AH22" s="21"/>
+      <c r="B22" s="76" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="64"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="58"/>
+      <c r="F22" s="58"/>
+      <c r="G22" s="58"/>
+      <c r="H22" s="77"/>
+      <c r="I22" s="77"/>
+      <c r="J22" s="77"/>
+      <c r="K22" s="77" t="s">
+        <v>113</v>
+      </c>
+      <c r="L22" s="150" t="s">
+        <v>117</v>
+      </c>
+      <c r="M22" s="151"/>
+      <c r="N22" s="151"/>
+      <c r="O22" s="151"/>
+      <c r="P22" s="151"/>
+      <c r="Q22" s="78"/>
+      <c r="R22" s="78"/>
+      <c r="S22" s="78"/>
+      <c r="T22" s="78"/>
+      <c r="U22" s="79"/>
+      <c r="V22" s="77"/>
+      <c r="W22" s="80" t="s">
+        <v>64</v>
+      </c>
+      <c r="X22" s="78"/>
+      <c r="Y22" s="78"/>
+      <c r="Z22" s="78"/>
+      <c r="AA22" s="78"/>
+      <c r="AB22" s="78"/>
+      <c r="AC22" s="78"/>
+      <c r="AD22" s="78"/>
+      <c r="AE22" s="78"/>
+      <c r="AF22" s="78"/>
+      <c r="AG22" s="78"/>
+      <c r="AH22" s="79"/>
       <c r="AI22" s="21"/>
     </row>
     <row r="23" spans="1:35" ht="24" customHeight="1">
@@ -3359,13 +3322,12 @@
       <c r="AH23" s="21"/>
       <c r="AI23" s="21"/>
     </row>
-    <row r="24" spans="1:35" ht="21" customHeight="1">
+    <row r="24" spans="1:35" ht="24" customHeight="1">
+      <c r="A24" s="19"/>
       <c r="B24" s="20"/>
-      <c r="C24" s="122" t="s">
-        <v>56</v>
-      </c>
-      <c r="D24" s="51"/>
-      <c r="E24" s="51"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
       <c r="F24" s="21"/>
       <c r="G24" s="21"/>
       <c r="H24" s="21"/>
@@ -3382,62 +3344,71 @@
       <c r="S24" s="21"/>
       <c r="T24" s="21"/>
       <c r="U24" s="21"/>
+      <c r="V24" s="21"/>
+      <c r="W24" s="21"/>
+      <c r="X24" s="21"/>
+      <c r="Y24" s="21"/>
+      <c r="Z24" s="21"/>
+      <c r="AA24" s="21"/>
+      <c r="AB24" s="21"/>
+      <c r="AC24" s="21"/>
+      <c r="AD24" s="21"/>
+      <c r="AE24" s="21"/>
+      <c r="AF24" s="21"/>
+      <c r="AG24" s="21"/>
+      <c r="AH24" s="21"/>
+      <c r="AI24" s="21"/>
     </row>
-    <row r="25" spans="1:35">
+    <row r="25" spans="1:35" ht="21" customHeight="1">
       <c r="B25" s="20"/>
-      <c r="C25" s="123" t="s">
-        <v>156</v>
-      </c>
-      <c r="D25" s="124"/>
-      <c r="E25" s="125" t="s">
-        <v>114</v>
-      </c>
-      <c r="F25" s="125"/>
-      <c r="G25" s="125"/>
-      <c r="H25" s="125"/>
-      <c r="I25" s="125"/>
-      <c r="J25" s="126" t="s">
-        <v>54</v>
-      </c>
-      <c r="K25" s="125"/>
-      <c r="L25" s="125"/>
-      <c r="M25" s="125"/>
-      <c r="N25" s="125"/>
-      <c r="O25" s="125"/>
-      <c r="P25" s="125"/>
-      <c r="Q25" s="125"/>
-      <c r="R25" s="125"/>
-      <c r="S25" s="125"/>
-      <c r="T25" s="124"/>
-      <c r="U25" s="22"/>
-      <c r="V25" s="6"/>
-      <c r="W25" s="6"/>
-      <c r="X25" s="6"/>
-      <c r="Y25" s="6"/>
-      <c r="Z25" s="6"/>
+      <c r="C25" s="122" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="51"/>
+      <c r="E25" s="51"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="21"/>
+      <c r="Q25" s="21"/>
+      <c r="R25" s="21"/>
+      <c r="S25" s="21"/>
+      <c r="T25" s="21"/>
+      <c r="U25" s="21"/>
     </row>
     <row r="26" spans="1:35">
       <c r="B26" s="20"/>
-      <c r="C26" s="127"/>
-      <c r="D26" s="128"/>
-      <c r="E26" s="129" t="s">
-        <v>113</v>
-      </c>
-      <c r="F26" s="129"/>
-      <c r="G26" s="129"/>
-      <c r="H26" s="129"/>
-      <c r="I26" s="129"/>
-      <c r="J26" s="130"/>
-      <c r="K26" s="131"/>
-      <c r="L26" s="131"/>
-      <c r="M26" s="131"/>
-      <c r="N26" s="131"/>
-      <c r="O26" s="131"/>
-      <c r="P26" s="131"/>
-      <c r="Q26" s="131"/>
-      <c r="R26" s="131"/>
-      <c r="S26" s="131"/>
-      <c r="T26" s="132"/>
+      <c r="C26" s="123" t="s">
+        <v>154</v>
+      </c>
+      <c r="D26" s="124"/>
+      <c r="E26" s="125" t="s">
+        <v>112</v>
+      </c>
+      <c r="F26" s="125"/>
+      <c r="G26" s="125"/>
+      <c r="H26" s="125"/>
+      <c r="I26" s="125"/>
+      <c r="J26" s="126" t="s">
+        <v>54</v>
+      </c>
+      <c r="K26" s="125"/>
+      <c r="L26" s="125"/>
+      <c r="M26" s="125"/>
+      <c r="N26" s="125"/>
+      <c r="O26" s="125"/>
+      <c r="P26" s="125"/>
+      <c r="Q26" s="125"/>
+      <c r="R26" s="125"/>
+      <c r="S26" s="125"/>
+      <c r="T26" s="124"/>
       <c r="U26" s="22"/>
       <c r="V26" s="6"/>
       <c r="W26" s="6"/>
@@ -3445,32 +3416,28 @@
       <c r="Y26" s="6"/>
       <c r="Z26" s="6"/>
     </row>
-    <row r="27" spans="1:35" ht="21" customHeight="1">
+    <row r="27" spans="1:35">
       <c r="B27" s="20"/>
-      <c r="C27" s="127" t="s">
-        <v>157</v>
-      </c>
+      <c r="C27" s="127"/>
       <c r="D27" s="128"/>
-      <c r="E27" s="131" t="s">
-        <v>52</v>
-      </c>
-      <c r="F27" s="131"/>
-      <c r="G27" s="131"/>
-      <c r="H27" s="131"/>
-      <c r="I27" s="131"/>
-      <c r="J27" s="126" t="s">
-        <v>55</v>
-      </c>
-      <c r="K27" s="125"/>
-      <c r="L27" s="125"/>
-      <c r="M27" s="125"/>
-      <c r="N27" s="125"/>
-      <c r="O27" s="125"/>
-      <c r="P27" s="125"/>
-      <c r="Q27" s="125"/>
-      <c r="R27" s="125"/>
-      <c r="S27" s="125"/>
-      <c r="T27" s="124"/>
+      <c r="E27" s="129" t="s">
+        <v>111</v>
+      </c>
+      <c r="F27" s="129"/>
+      <c r="G27" s="129"/>
+      <c r="H27" s="129"/>
+      <c r="I27" s="129"/>
+      <c r="J27" s="130"/>
+      <c r="K27" s="131"/>
+      <c r="L27" s="131"/>
+      <c r="M27" s="131"/>
+      <c r="N27" s="131"/>
+      <c r="O27" s="131"/>
+      <c r="P27" s="131"/>
+      <c r="Q27" s="131"/>
+      <c r="R27" s="131"/>
+      <c r="S27" s="131"/>
+      <c r="T27" s="132"/>
       <c r="U27" s="22"/>
       <c r="V27" s="6"/>
       <c r="W27" s="6"/>
@@ -3480,19 +3447,19 @@
     </row>
     <row r="28" spans="1:35" ht="21" customHeight="1">
       <c r="B28" s="20"/>
-      <c r="C28" s="133" t="s">
-        <v>158</v>
-      </c>
-      <c r="D28" s="134"/>
-      <c r="E28" s="153" t="s">
-        <v>161</v>
-      </c>
-      <c r="F28" s="147"/>
-      <c r="G28" s="147"/>
-      <c r="H28" s="147"/>
-      <c r="I28" s="147"/>
+      <c r="C28" s="127" t="s">
+        <v>155</v>
+      </c>
+      <c r="D28" s="128"/>
+      <c r="E28" s="131" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" s="131"/>
+      <c r="G28" s="131"/>
+      <c r="H28" s="131"/>
+      <c r="I28" s="131"/>
       <c r="J28" s="126" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="K28" s="125"/>
       <c r="L28" s="125"/>
@@ -3512,18 +3479,18 @@
       <c r="Z28" s="6"/>
     </row>
     <row r="29" spans="1:35" ht="21" customHeight="1">
-      <c r="B29" s="44"/>
-      <c r="C29" s="135" t="s">
+      <c r="B29" s="20"/>
+      <c r="C29" s="133" t="s">
+        <v>156</v>
+      </c>
+      <c r="D29" s="134"/>
+      <c r="E29" s="155" t="s">
         <v>159</v>
       </c>
-      <c r="D29" s="134"/>
-      <c r="E29" s="148" t="s">
-        <v>79</v>
-      </c>
-      <c r="F29" s="148"/>
-      <c r="G29" s="148"/>
-      <c r="H29" s="148"/>
-      <c r="I29" s="148"/>
+      <c r="F29" s="153"/>
+      <c r="G29" s="153"/>
+      <c r="H29" s="153"/>
+      <c r="I29" s="153"/>
       <c r="J29" s="126" t="s">
         <v>53</v>
       </c>
@@ -3545,31 +3512,31 @@
       <c r="Z29" s="6"/>
     </row>
     <row r="30" spans="1:35" ht="21" customHeight="1">
-      <c r="B30" s="20"/>
-      <c r="C30" s="133" t="s">
-        <v>160</v>
+      <c r="B30" s="44"/>
+      <c r="C30" s="135" t="s">
+        <v>157</v>
       </c>
       <c r="D30" s="134"/>
-      <c r="E30" s="146" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30" s="147"/>
-      <c r="G30" s="147"/>
-      <c r="H30" s="147"/>
-      <c r="I30" s="147"/>
-      <c r="J30" s="136" t="s">
-        <v>51</v>
-      </c>
-      <c r="K30" s="137"/>
-      <c r="L30" s="137"/>
-      <c r="M30" s="137"/>
-      <c r="N30" s="137"/>
-      <c r="O30" s="137"/>
-      <c r="P30" s="137"/>
-      <c r="Q30" s="137"/>
-      <c r="R30" s="137"/>
-      <c r="S30" s="137"/>
-      <c r="T30" s="134"/>
+      <c r="E30" s="154" t="s">
+        <v>77</v>
+      </c>
+      <c r="F30" s="154"/>
+      <c r="G30" s="154"/>
+      <c r="H30" s="154"/>
+      <c r="I30" s="154"/>
+      <c r="J30" s="126" t="s">
+        <v>53</v>
+      </c>
+      <c r="K30" s="125"/>
+      <c r="L30" s="125"/>
+      <c r="M30" s="125"/>
+      <c r="N30" s="125"/>
+      <c r="O30" s="125"/>
+      <c r="P30" s="125"/>
+      <c r="Q30" s="125"/>
+      <c r="R30" s="125"/>
+      <c r="S30" s="125"/>
+      <c r="T30" s="124"/>
       <c r="U30" s="22"/>
       <c r="V30" s="6"/>
       <c r="W30" s="6"/>
@@ -3577,27 +3544,38 @@
       <c r="Y30" s="6"/>
       <c r="Z30" s="6"/>
     </row>
-    <row r="31" spans="1:35" ht="17.100000000000001" customHeight="1">
+    <row r="31" spans="1:35" ht="21" customHeight="1">
       <c r="B31" s="20"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21"/>
-      <c r="K31" s="21"/>
-      <c r="L31" s="21"/>
-      <c r="M31" s="21"/>
-      <c r="N31" s="21"/>
-      <c r="O31" s="21"/>
-      <c r="P31" s="21"/>
-      <c r="Q31" s="21"/>
-      <c r="R31" s="21"/>
-      <c r="S31" s="21"/>
-      <c r="T31" s="21"/>
-      <c r="U31" s="21"/>
+      <c r="C31" s="133" t="s">
+        <v>158</v>
+      </c>
+      <c r="D31" s="134"/>
+      <c r="E31" s="152" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="153"/>
+      <c r="G31" s="153"/>
+      <c r="H31" s="153"/>
+      <c r="I31" s="153"/>
+      <c r="J31" s="136" t="s">
+        <v>51</v>
+      </c>
+      <c r="K31" s="137"/>
+      <c r="L31" s="137"/>
+      <c r="M31" s="137"/>
+      <c r="N31" s="137"/>
+      <c r="O31" s="137"/>
+      <c r="P31" s="137"/>
+      <c r="Q31" s="137"/>
+      <c r="R31" s="137"/>
+      <c r="S31" s="137"/>
+      <c r="T31" s="134"/>
+      <c r="U31" s="22"/>
+      <c r="V31" s="6"/>
+      <c r="W31" s="6"/>
+      <c r="X31" s="6"/>
+      <c r="Y31" s="6"/>
+      <c r="Z31" s="6"/>
     </row>
     <row r="32" spans="1:35" ht="17.100000000000001" customHeight="1">
       <c r="B32" s="20"/>
@@ -3621,78 +3599,100 @@
       <c r="T32" s="21"/>
       <c r="U32" s="21"/>
     </row>
+    <row r="33" spans="2:21" ht="17.100000000000001" customHeight="1">
+      <c r="B33" s="20"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="21"/>
+      <c r="L33" s="21"/>
+      <c r="M33" s="21"/>
+      <c r="N33" s="21"/>
+      <c r="O33" s="21"/>
+      <c r="P33" s="21"/>
+      <c r="Q33" s="21"/>
+      <c r="R33" s="21"/>
+      <c r="S33" s="21"/>
+      <c r="T33" s="21"/>
+      <c r="U33" s="21"/>
+    </row>
   </sheetData>
   <mergeCells count="70">
+    <mergeCell ref="E31:I31"/>
     <mergeCell ref="E30:I30"/>
     <mergeCell ref="E29:I29"/>
-    <mergeCell ref="E28:I28"/>
-    <mergeCell ref="L10:O10"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="L8:P8"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="L3:O3"/>
-    <mergeCell ref="L21:P21"/>
-    <mergeCell ref="Y20:Z20"/>
-    <mergeCell ref="AA20:AB20"/>
-    <mergeCell ref="AC20:AD20"/>
-    <mergeCell ref="AE20:AF20"/>
-    <mergeCell ref="AG20:AH20"/>
-    <mergeCell ref="L20:O20"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="R20:S20"/>
-    <mergeCell ref="T20:U20"/>
-    <mergeCell ref="W20:X20"/>
-    <mergeCell ref="Y16:Z16"/>
-    <mergeCell ref="AA16:AB16"/>
-    <mergeCell ref="AC16:AD16"/>
-    <mergeCell ref="AE16:AF16"/>
-    <mergeCell ref="AG16:AH16"/>
-    <mergeCell ref="L16:O16"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="T16:U16"/>
-    <mergeCell ref="W16:X16"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="R10:S10"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="T7:U7"/>
-    <mergeCell ref="W7:X7"/>
-    <mergeCell ref="Y7:Z7"/>
-    <mergeCell ref="AA7:AB7"/>
-    <mergeCell ref="AC7:AD7"/>
-    <mergeCell ref="AE7:AF7"/>
-    <mergeCell ref="AG7:AH7"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="Y3:Z3"/>
-    <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="AC3:AD3"/>
-    <mergeCell ref="AE3:AF3"/>
-    <mergeCell ref="AG14:AH14"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="L14:O14"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="R14:S14"/>
-    <mergeCell ref="T14:U14"/>
-    <mergeCell ref="W14:X14"/>
-    <mergeCell ref="Y14:Z14"/>
-    <mergeCell ref="AA14:AB14"/>
-    <mergeCell ref="AC14:AD14"/>
-    <mergeCell ref="AE14:AF14"/>
-    <mergeCell ref="T10:U10"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="AA10:AB10"/>
-    <mergeCell ref="AC10:AD10"/>
-    <mergeCell ref="AE10:AF10"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="AG10:AH10"/>
-    <mergeCell ref="AG3:AH3"/>
-    <mergeCell ref="L7:O7"/>
-    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="L11:O11"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="L22:P22"/>
+    <mergeCell ref="L21:O21"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="AE21:AF21"/>
+    <mergeCell ref="AG21:AH21"/>
+    <mergeCell ref="L9:P9"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="T21:U21"/>
+    <mergeCell ref="W21:X21"/>
+    <mergeCell ref="Y17:Z17"/>
+    <mergeCell ref="AA17:AB17"/>
+    <mergeCell ref="AC17:AD17"/>
+    <mergeCell ref="Y21:Z21"/>
+    <mergeCell ref="AA21:AB21"/>
+    <mergeCell ref="AC21:AD21"/>
+    <mergeCell ref="L17:O17"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="T17:U17"/>
+    <mergeCell ref="W17:X17"/>
+    <mergeCell ref="Y8:Z8"/>
+    <mergeCell ref="AA8:AB8"/>
+    <mergeCell ref="AC8:AD8"/>
+    <mergeCell ref="AE17:AF17"/>
+    <mergeCell ref="AG17:AH17"/>
+    <mergeCell ref="AG15:AH15"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="L15:O15"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="R15:S15"/>
+    <mergeCell ref="T15:U15"/>
+    <mergeCell ref="W15:X15"/>
+    <mergeCell ref="Y15:Z15"/>
+    <mergeCell ref="AA15:AB15"/>
+    <mergeCell ref="AC15:AD15"/>
+    <mergeCell ref="AE15:AF15"/>
+    <mergeCell ref="T11:U11"/>
+    <mergeCell ref="W11:X11"/>
+    <mergeCell ref="Y11:Z11"/>
+    <mergeCell ref="AA11:AB11"/>
+    <mergeCell ref="AC11:AD11"/>
+    <mergeCell ref="AE11:AF11"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="AG11:AH11"/>
+    <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="L8:O8"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="AE8:AF8"/>
+    <mergeCell ref="AG8:AH8"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="AA4:AB4"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="T8:U8"/>
+    <mergeCell ref="W8:X8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>